<commit_message>
commit for func urmin (js, controller, view)
</commit_message>
<xml_diff>
--- a/assets/excel/import_data.xlsx
+++ b/assets/excel/import_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Documents\Informatika UNDIP\PKL-- cayooo\--FILE--\FORMAT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDE64612-60F4-4FC8-B24F-3199864C61E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E542F4B9-3759-4480-9268-C0204869C526}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2620" yWindow="2620" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
   <si>
     <t>NAMA</t>
   </si>
@@ -64,37 +64,34 @@
     <t>ID_BAGIAN</t>
   </si>
   <si>
-    <t>ARDI ARYA SAMUDRA</t>
-  </si>
-  <si>
-    <t>BRIPTU</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ADMINISTRASI </t>
-  </si>
-  <si>
-    <t>TEGAL</t>
+    <t>KOMPOL</t>
+  </si>
+  <si>
+    <t>ADMINISTRASI</t>
+  </si>
+  <si>
+    <t>PEKALONGAN</t>
+  </si>
+  <si>
+    <t>SEMARANG</t>
   </si>
   <si>
     <t>KRISTEN</t>
   </si>
   <si>
+    <t>ISLAM</t>
+  </si>
+  <si>
     <t>JAWA</t>
   </si>
   <si>
-    <t>ANJAR HARYONO KUSUMO</t>
-  </si>
-  <si>
-    <t>BRIGADIR</t>
-  </si>
-  <si>
-    <t>PENGDA II</t>
-  </si>
-  <si>
-    <t>SEMARANG</t>
-  </si>
-  <si>
-    <t>ISLAM</t>
+    <t>BUGIS</t>
+  </si>
+  <si>
+    <t>ANDI SURANA</t>
+  </si>
+  <si>
+    <t>MURNIATI</t>
   </si>
 </sst>
 </file>
@@ -104,7 +101,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -112,43 +109,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF333333"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -156,43 +126,16 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFEEEEEE"/>
-      </left>
-      <right style="medium">
-        <color rgb="FFEEEEEE"/>
-      </right>
-      <top style="medium">
-        <color rgb="FFEEEEEE"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FFEEEEEE"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -532,7 +475,7 @@
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:J3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -550,7 +493,7 @@
     <col min="11" max="11" width="13" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -582,68 +525,68 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="1">
+        <v>12312216</v>
+      </c>
+      <c r="C2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="4">
-        <v>87121310</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>11</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>12</v>
       </c>
-      <c r="E2" t="s">
-        <v>13</v>
-      </c>
       <c r="F2" s="2">
-        <v>31947</v>
+        <v>36210</v>
       </c>
       <c r="G2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I2" s="2">
-        <v>43831</v>
+        <v>43862</v>
       </c>
       <c r="J2" s="1">
-        <v>20</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A3" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" s="6">
-        <v>77311213</v>
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="1">
+        <v>12121768</v>
       </c>
       <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="2">
+        <v>36201</v>
+      </c>
+      <c r="G3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" t="s">
         <v>17</v>
       </c>
-      <c r="D3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F3" s="2">
-        <v>28477</v>
-      </c>
-      <c r="G3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H3" t="s">
-        <v>15</v>
-      </c>
       <c r="I3" s="2">
-        <v>43831</v>
+        <v>43862</v>
       </c>
       <c r="J3" s="1">
-        <v>21</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>